<commit_message>
Material change drawing revision to v1.1 rev B
Revised LEDCON.FACE and LEDCON.BACK to v1.1 rev B, material changed to
6061 Aluminum. ECO also updated.
</commit_message>
<xml_diff>
--- a/LEDCON.MECH.ECO.xlsx
+++ b/LEDCON.MECH.ECO.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
   <si>
     <t>Release ID</t>
   </si>
@@ -69,6 +72,15 @@
   <si>
     <t>Reset button added to daughterboard, needed a slot cut in the core part 
 CORESIDE part split off from COREMID/COREBOT drawings to reduce confusion and simplify production going forward</t>
+  </si>
+  <si>
+    <t>LEDCON.MECH.v1.2</t>
+  </si>
+  <si>
+    <t>Material changed to 6061 Aluminum</t>
+  </si>
+  <si>
+    <t>Material change initiated by supplier, improvement in anodizability</t>
   </si>
 </sst>
 </file>
@@ -78,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -95,12 +107,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -108,12 +125,12 @@
       <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,10 +141,56 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -147,32 +210,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -209,7 +306,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>492427</xdr:colOff>
+      <xdr:colOff>530526</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>394335</xdr:rowOff>
     </xdr:to>
@@ -220,8 +317,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="-133350"/>
-          <a:ext cx="4289728" cy="394336"/>
+          <a:off x="0" y="-1"/>
+          <a:ext cx="5648627" cy="394336"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1507,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:K14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1522,227 +1619,262 @@
     <col min="7" max="7" width="13.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.25" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="40.2188" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1" customWidth="1"/>
     <col min="12" max="256" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.95" customHeight="1"/>
+    <row r="1" ht="31.95" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+    </row>
     <row r="2" ht="18" customHeight="1">
-      <c r="B2" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s" s="2">
+      <c r="A2" s="5"/>
+      <c r="B2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="C2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="D2" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="E2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="F2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="G2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="I2" t="s" s="2">
+      <c r="H2" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="J2" t="s" s="2">
+      <c r="I2" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="K2" t="s" s="2">
+      <c r="J2" t="s" s="6">
         <v>9</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="31" customHeight="1">
-      <c r="B3" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="3">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s" s="3">
+      <c r="C3" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="H3" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s" s="3">
+      <c r="D3" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="J3" t="s" s="4">
+      <c r="H3" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="K3" s="5">
+      <c r="J3" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="K3" s="9">
         <v>42066</v>
       </c>
     </row>
-    <row r="4" ht="70" customHeight="1">
-      <c r="B4" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s" s="4">
+    <row r="4" ht="82.2" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="F4" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s" s="4">
+      <c r="C4" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="8">
         <v>17</v>
       </c>
-      <c r="H4" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s" s="4">
+      <c r="F4" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="K4" s="5">
+      <c r="H4" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="K4" s="9">
         <v>42100</v>
       </c>
     </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+    <row r="5" ht="47.8" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" ht="18" customHeight="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" ht="18" customHeight="1">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" ht="18" customHeight="1">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" ht="18" customHeight="1">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" ht="18" customHeight="1">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" ht="18" customHeight="1">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" ht="18" customHeight="1">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" ht="18" customHeight="1">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added line for v1.3
</commit_message>
<xml_diff>
--- a/LEDCON.MECH.ECO.xlsx
+++ b/LEDCON.MECH.ECO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -81,14 +81,24 @@
   </si>
   <si>
     <t>Material change initiated by supplier, improvement in anodizability</t>
+  </si>
+  <si>
+    <t>LEDCON.MECH.v1.3</t>
+  </si>
+  <si>
+    <t>Added BOM</t>
+  </si>
+  <si>
+    <t>Subassembly requires its own BOM (value add)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -229,7 +239,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -239,13 +249,13 @@
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -260,16 +270,19 @@
     <xf numFmtId="14" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="59" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="1" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -306,7 +319,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>530526</xdr:colOff>
+      <xdr:colOff>568626</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>394335</xdr:rowOff>
     </xdr:to>
@@ -317,8 +330,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="-1"/>
-          <a:ext cx="5648627" cy="394336"/>
+          <a:off x="-1" y="-1"/>
+          <a:ext cx="5686728" cy="394336"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1746,10 +1759,18 @@
       <c r="C5" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="D5" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s" s="7">
+        <v>12</v>
+      </c>
       <c r="H5" t="s" s="8">
         <v>21</v>
       </c>
@@ -1761,120 +1782,140 @@
     </row>
     <row r="6" ht="18" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="B6" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="K6" s="12">
+        <v>42129</v>
+      </c>
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" ht="18" customHeight="1">
       <c r="A8" s="5"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" ht="18" customHeight="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" ht="18" customHeight="1">
       <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" ht="18" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" ht="18" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" ht="18" customHeight="1">
       <c r="A13" s="5"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added 0.031" radius to notches on back of faceplate to reduce potential confusion with vendor
</commit_message>
<xml_diff>
--- a/LEDCON.MECH.ECO.xlsx
+++ b/LEDCON.MECH.ECO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t> </t>
   </si>
@@ -157,16 +157,26 @@
   </si>
   <si>
     <t>Filename changes for clarity</t>
+  </si>
+  <si>
+    <t>LEDCON.MECH.v1.5</t>
+  </si>
+  <si>
+    <t>Added 0.031” radius to notches on back of faceplate</t>
+  </si>
+  <si>
+    <t>Radius added to drawings to reduce potential vendor confusion (first articles &amp; subsequent production items from vendor had radiused corners in the notches)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -260,7 +270,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,6 +295,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,6 +308,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -314,27 +332,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.8111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.3259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.7518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.9444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.8185185185185"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.75555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.0740740740741"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.0037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.537037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.8111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.9925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.6888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.7851851851852"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.62962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.0666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -391,11 +409,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
@@ -420,7 +439,7 @@
       <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="6" t="n">
+      <c r="L3" s="7" t="n">
         <v>42066</v>
       </c>
     </row>
@@ -429,6 +448,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
@@ -453,7 +473,7 @@
       <c r="K4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="6" t="n">
+      <c r="L4" s="7" t="n">
         <v>42100</v>
       </c>
     </row>
@@ -462,6 +482,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
@@ -522,7 +543,7 @@
       <c r="K6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L6" s="7" t="n">
         <v>42129</v>
       </c>
     </row>
@@ -531,6 +552,7 @@
       <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -539,13 +561,14 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="6"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -554,13 +577,14 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="6"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -569,13 +593,14 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="6"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -584,13 +609,14 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="6"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -599,13 +625,14 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="6"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -614,13 +641,14 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="6"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="C13" s="6"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -629,13 +657,14 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="6"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="C14" s="6"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -644,13 +673,14 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="6"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -659,13 +689,14 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="6"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C16" s="6"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -674,13 +705,14 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C17" s="6"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -689,13 +721,14 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="6"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="C18" s="6"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -704,15 +737,16 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="6"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="58.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
@@ -737,13 +771,13 @@
       <c r="K19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L19" s="6" t="n">
+      <c r="L19" s="7" t="n">
         <v>42201</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="3"/>
@@ -759,7 +793,7 @@
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="3"/>
@@ -789,10 +823,42 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
+    <row r="23" customFormat="false" ht="60.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>42256</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1.16666666666667" bottom="1" header="1" footer="0.5"/>
-  <pageSetup paperSize="1" scale="45" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;"Times New Roman,Regular"LEDCON.MECH.ECO</oddHeader>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>

</xml_diff>

<commit_message>
Changes to BOM & ECO reverted. Ignore previous commit. Changes were intended for POSCON.FACE
</commit_message>
<xml_diff>
--- a/LEDCON.MECH.ECO.xlsx
+++ b/LEDCON.MECH.ECO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t> </t>
   </si>
@@ -157,26 +157,16 @@
   </si>
   <si>
     <t>Filename changes for clarity</t>
-  </si>
-  <si>
-    <t>LEDCON.MECH.v1.5</t>
-  </si>
-  <si>
-    <t>Added 0.031” radius to notches on back of faceplate</t>
-  </si>
-  <si>
-    <t>Radius added to drawings to reduce potential vendor confusion (first articles &amp; subsequent production items from vendor had radiused corners in the notches)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -275,43 +265,43 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,27 +322,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.537037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.5666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.8111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.9925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.6888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.7851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.62962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.9518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.9259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.7185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.5407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.6666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.9962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.1851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.5962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.32222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="15.1888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -516,7 +506,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -743,7 +733,7 @@
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="6"/>
@@ -777,7 +767,7 @@
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="3"/>
@@ -793,7 +783,7 @@
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="3"/>
@@ -823,38 +813,6 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="60.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L23" s="10" t="n">
-        <v>42256</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1.16666666666667" bottom="1" header="1" footer="0.5"/>

</xml_diff>